<commit_message>
Refresh And New Row
</commit_message>
<xml_diff>
--- a/thesis_data.xlsx
+++ b/thesis_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QR Project\V0\QRScannerService\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A270A40F-C7AD-46F8-9C5C-832D607CDD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD88C21D-4543-47F1-A71D-3367D1B0622D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="684" windowWidth="11712" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="108" yWindow="168" windowWidth="11712" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
     <t>isfahan</t>
   </si>
   <si>
-    <t>nicht zugelassen</t>
+    <t>zugelassen</t>
   </si>
   <si>
-    <t>umr-fb12-finalthesis_1.0_2024-10-31</t>
+    <t>umr-fb12-finalthesis_1.0.1_2025-02-06</t>
   </si>
 </sst>
 </file>
@@ -358,7 +358,7 @@
   <dimension ref="J1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="D1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -386,7 +386,7 @@
         <v>0</v>
       </c>
       <c r="Q1" s="1">
-        <v>45627</v>
+        <v>36861</v>
       </c>
       <c r="R1" t="s">
         <v>1</v>

</xml_diff>